<commit_message>
update list of spreads
</commit_message>
<xml_diff>
--- a/data/OI_product_map.xlsx
+++ b/data/OI_product_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hoteicapital-my.sharepoint.com/personal/jiashang_hoteicapital_com/Documents/Desktop/Notebooks/Streamlit_v1/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="8_{A4D98350-709A-462B-87D2-DA567DEA5457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B6FB77D-6365-4B1C-B3C8-2D9E7E4381F9}"/>
+  <xr:revisionPtr revIDLastSave="115" documentId="8_{A4D98350-709A-462B-87D2-DA567DEA5457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31A1ABFB-B8A1-4CCD-8911-E88A0CFFAED8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{542C41B4-5129-4961-BD89-52D58DBA0F0A}"/>
+    <workbookView xWindow="4965" yWindow="1350" windowWidth="26700" windowHeight="12615" xr2:uid="{542C41B4-5129-4961-BD89-52D58DBA0F0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -809,10 +809,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A59FE1-DE17-4881-8BC1-F91F83F8F9F7}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,11 +874,11 @@
         <v>74</v>
       </c>
       <c r="H2" t="str">
-        <f>_xlfn.CONCAT(D2," (",G2, ")")</f>
+        <f t="shared" ref="H2:H33" si="0">_xlfn.CONCAT(D2," (",G2, ")")</f>
         <v>SMT (Singapore Mogas 92 Unleaded Swap)</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -885,14 +886,14 @@
         <v>5</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C63" si="0">_xlfn.CONCAT("[",A3,"] ",B3)</f>
+        <f t="shared" ref="C3:C63" si="1">_xlfn.CONCAT("[",A3,"] ",B3)</f>
         <v>[Light] S92</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E63" si="1">_xlfn.CONCAT("'",D3,"',")</f>
+        <f t="shared" ref="E3:E63" si="2">_xlfn.CONCAT("'",D3,"',")</f>
         <v>'GDK',</v>
       </c>
       <c r="F3">
@@ -902,11 +903,11 @@
         <v>75</v>
       </c>
       <c r="H3" t="str">
-        <f>_xlfn.CONCAT(D3," (",G3, ")")</f>
+        <f t="shared" si="0"/>
         <v>GDK (Gasoline Diff - Singapore Mogas 92 Unleaded (Platts) vs Argus Eurobob Oxy FOB Rotterdam Barges Future)</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -914,14 +915,14 @@
         <v>5</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Light] S92</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'STB',</v>
       </c>
       <c r="F4">
@@ -931,7 +932,7 @@
         <v>76</v>
       </c>
       <c r="H4" t="str">
-        <f>_xlfn.CONCAT(D4," (",G4, ")")</f>
+        <f t="shared" si="0"/>
         <v>STB (Singapore Mogas 92 Unleaded vs Brent 1st Line Future)</v>
       </c>
     </row>
@@ -943,14 +944,14 @@
         <v>9</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Light] Ebob</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'AEO',</v>
       </c>
       <c r="F5">
@@ -960,11 +961,11 @@
         <v>11</v>
       </c>
       <c r="H5" t="str">
-        <f>_xlfn.CONCAT(D5," (",G5, ")")</f>
+        <f t="shared" si="0"/>
         <v>AEO (Argus Eurobob Oxy FOB Rotterdam Barges Future)</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -972,14 +973,14 @@
         <v>9</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Light] Ebob</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'GDK',</v>
       </c>
       <c r="F6">
@@ -989,11 +990,11 @@
         <v>75</v>
       </c>
       <c r="H6" t="str">
-        <f>_xlfn.CONCAT(D6," (",G6, ")")</f>
+        <f t="shared" si="0"/>
         <v>GDK (Gasoline Diff - Singapore Mogas 92 Unleaded (Platts) vs Argus Eurobob Oxy FOB Rotterdam Barges Future)</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1001,14 +1002,14 @@
         <v>9</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Light] Ebob</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'EOB',</v>
       </c>
       <c r="F7">
@@ -1018,11 +1019,11 @@
         <v>77</v>
       </c>
       <c r="H7" t="str">
-        <f>_xlfn.CONCAT(D7," (",G7, ")")</f>
+        <f t="shared" si="0"/>
         <v>EOB (Gasoline Crack - Argus Eurobob Oxy FOB Rotterdam Barges vs Brent 1st Line Future)</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1030,14 +1031,14 @@
         <v>9</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Light] Ebob</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'GDO',</v>
       </c>
       <c r="F8">
@@ -1047,11 +1048,11 @@
         <v>78</v>
       </c>
       <c r="H8" t="str">
-        <f>_xlfn.CONCAT(D8," (",G8, ")")</f>
+        <f t="shared" si="0"/>
         <v>GDO (Gasoline Diff - RBOB Gasoline 1st Line vs Argus Eurobob Oxy FOB Rotterdam Barge Future)</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1059,24 +1060,24 @@
         <v>9</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Light] Ebob</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'EON',</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" t="s">
         <v>79</v>
       </c>
       <c r="H9" t="str">
-        <f>_xlfn.CONCAT(D9," (",G9, ")")</f>
+        <f t="shared" si="0"/>
         <v>EON (Argus Eurobob OXY FOB Rotterdam Barges VS Platts Naphtha CIF NWE Cargoes Future)</v>
       </c>
     </row>
@@ -1088,14 +1089,14 @@
         <v>15</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Light] Rbob</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'UHU',</v>
       </c>
       <c r="F10" s="1">
@@ -1105,7 +1106,7 @@
         <v>80</v>
       </c>
       <c r="H10" t="str">
-        <f>_xlfn.CONCAT(D10," (",G10, ")")</f>
+        <f t="shared" si="0"/>
         <v>UHU (NYH (RBOB) Gasoline Futures)</v>
       </c>
     </row>
@@ -1117,14 +1118,14 @@
         <v>15</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Light] Rbob</v>
       </c>
       <c r="D11" t="s">
         <v>17</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'RBS',</v>
       </c>
       <c r="F11">
@@ -1134,11 +1135,11 @@
         <v>81</v>
       </c>
       <c r="H11" t="str">
-        <f>_xlfn.CONCAT(D11," (",G11, ")")</f>
+        <f t="shared" si="0"/>
         <v>RBS (RBOB Gasoline 1st Line Future)</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1146,14 +1147,14 @@
         <v>15</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Light] Rbob</v>
       </c>
       <c r="D12" t="s">
         <v>18</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'RBR',</v>
       </c>
       <c r="F12">
@@ -1163,11 +1164,11 @@
         <v>82</v>
       </c>
       <c r="H12" t="str">
-        <f>_xlfn.CONCAT(D12," (",G12, ")")</f>
+        <f t="shared" si="0"/>
         <v>RBR (Gasoline Crack - RBOB Gasoline 1st Line vs Brent 1st Line Future (in bbls))</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1175,14 +1176,14 @@
         <v>15</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Light] Rbob</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'GDO',</v>
       </c>
       <c r="F13">
@@ -1192,7 +1193,7 @@
         <v>78</v>
       </c>
       <c r="H13" t="str">
-        <f>_xlfn.CONCAT(D13," (",G13, ")")</f>
+        <f t="shared" si="0"/>
         <v>GDO (Gasoline Diff - RBOB Gasoline 1st Line vs Argus Eurobob Oxy FOB Rotterdam Barge Future)</v>
       </c>
     </row>
@@ -1204,14 +1205,14 @@
         <v>19</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Light] MOPJ Naph</v>
       </c>
       <c r="D14" t="s">
         <v>20</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'NJC',</v>
       </c>
       <c r="F14">
@@ -1221,11 +1222,11 @@
         <v>83</v>
       </c>
       <c r="H14" t="str">
-        <f>_xlfn.CONCAT(D14," (",G14, ")")</f>
+        <f t="shared" si="0"/>
         <v>NJC (Naphtha C+F Japan Cargo Swap)</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1233,14 +1234,14 @@
         <v>19</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Light] MOPJ Naph</v>
       </c>
       <c r="D15" t="s">
         <v>21</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'NBG',</v>
       </c>
       <c r="F15">
@@ -1250,11 +1251,11 @@
         <v>84</v>
       </c>
       <c r="H15" t="str">
-        <f>_xlfn.CONCAT(D15," (",G15, ")")</f>
+        <f t="shared" si="0"/>
         <v>NBG (Naphtha Crack - Naphtha C+F Japan (Platts) vs Brent 1st Line Future (in Bbls))</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1262,14 +1263,14 @@
         <v>19</v>
       </c>
       <c r="C16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Light] MOPJ Naph</v>
       </c>
       <c r="D16" t="s">
         <v>22</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'JOE',</v>
       </c>
       <c r="F16">
@@ -1279,7 +1280,7 @@
         <v>85</v>
       </c>
       <c r="H16" t="str">
-        <f>_xlfn.CONCAT(D16," (",G16, ")")</f>
+        <f t="shared" si="0"/>
         <v>JOE (Naphtha Diff - Naphtha C+F Japan vs Naphtha CIF NWE Cargoes Future)</v>
       </c>
     </row>
@@ -1291,14 +1292,14 @@
         <v>23</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Light] NWE Naph</v>
       </c>
       <c r="D17" t="s">
         <v>24</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'NEC',</v>
       </c>
       <c r="F17">
@@ -1308,11 +1309,11 @@
         <v>86</v>
       </c>
       <c r="H17" t="str">
-        <f>_xlfn.CONCAT(D17," (",G17, ")")</f>
+        <f t="shared" si="0"/>
         <v>NEC (Naphtha CIF NWE Cargoes Swap)</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1320,14 +1321,14 @@
         <v>23</v>
       </c>
       <c r="C18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Light] NWE Naph</v>
       </c>
       <c r="D18" t="s">
         <v>22</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'JOE',</v>
       </c>
       <c r="F18">
@@ -1337,11 +1338,11 @@
         <v>85</v>
       </c>
       <c r="H18" t="str">
-        <f>_xlfn.CONCAT(D18," (",G18, ")")</f>
+        <f t="shared" si="0"/>
         <v>JOE (Naphtha Diff - Naphtha C+F Japan vs Naphtha CIF NWE Cargoes Future)</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1349,14 +1350,14 @@
         <v>23</v>
       </c>
       <c r="C19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Light] NWE Naph</v>
       </c>
       <c r="D19" t="s">
         <v>25</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'NOB',</v>
       </c>
       <c r="F19">
@@ -1366,11 +1367,11 @@
         <v>87</v>
       </c>
       <c r="H19" t="str">
-        <f>_xlfn.CONCAT(D19," (",G19, ")")</f>
+        <f t="shared" si="0"/>
         <v>NOB (Naphtha CIF NWE Cargoes vs Brent 1st Line Swap)</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1378,14 +1379,14 @@
         <v>23</v>
       </c>
       <c r="C20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Light] NWE Naph</v>
       </c>
       <c r="D20" t="s">
         <v>14</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'EON',</v>
       </c>
       <c r="F20">
@@ -1395,11 +1396,11 @@
         <v>79</v>
       </c>
       <c r="H20" t="str">
-        <f>_xlfn.CONCAT(D20," (",G20, ")")</f>
+        <f t="shared" si="0"/>
         <v>EON (Argus Eurobob OXY FOB Rotterdam Barges VS Platts Naphtha CIF NWE Cargoes Future)</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1407,14 +1408,14 @@
         <v>27</v>
       </c>
       <c r="C21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Middle] SGO</v>
       </c>
       <c r="D21" t="s">
         <v>28</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'GST.J',</v>
       </c>
       <c r="F21">
@@ -1424,11 +1425,11 @@
         <v>88</v>
       </c>
       <c r="H21" t="str">
-        <f>_xlfn.CONCAT(D21," (",G21, ")")</f>
+        <f t="shared" si="0"/>
         <v>GST.J (Singapore Gasoil Swap)</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1436,14 +1437,14 @@
         <v>27</v>
       </c>
       <c r="C22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Middle] SGO</v>
       </c>
       <c r="D22" t="s">
         <v>29</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'SGB',</v>
       </c>
       <c r="F22">
@@ -1453,11 +1454,11 @@
         <v>89</v>
       </c>
       <c r="H22" t="str">
-        <f>_xlfn.CONCAT(D22," (",G22, ")")</f>
+        <f t="shared" si="0"/>
         <v>SGB (Gasoil Crack - Singapore Gasoil (Platts) vs Brent 1st Line Future)</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1465,14 +1466,14 @@
         <v>27</v>
       </c>
       <c r="C23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Middle] SGO</v>
       </c>
       <c r="D23" t="s">
         <v>30</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'BAO',</v>
       </c>
       <c r="F23">
@@ -1482,11 +1483,11 @@
         <v>90</v>
       </c>
       <c r="H23" t="str">
-        <f>_xlfn.CONCAT(D23," (",G23, ")")</f>
+        <f t="shared" si="0"/>
         <v>BAO (Gasoil Crack - Singapore Gasoil (Platts) vs Dubai 1st Line (Platts) Future)</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1494,14 +1495,14 @@
         <v>27</v>
       </c>
       <c r="C24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Middle] SGO</v>
       </c>
       <c r="D24" t="s">
         <v>31</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'BAP',</v>
       </c>
       <c r="F24">
@@ -1511,11 +1512,11 @@
         <v>91</v>
       </c>
       <c r="H24" t="str">
-        <f>_xlfn.CONCAT(D24," (",G24, ")")</f>
+        <f t="shared" si="0"/>
         <v>BAP (Gasoil Diff - Singapore Gasoil (Platts) vs Low Sulphur Gasoil 1st Line Future (in Bbls))</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1523,14 +1524,14 @@
         <v>27</v>
       </c>
       <c r="C25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Middle] SGO</v>
       </c>
       <c r="D25" t="s">
         <v>32</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'BAQ',</v>
       </c>
       <c r="F25">
@@ -1540,11 +1541,11 @@
         <v>92</v>
       </c>
       <c r="H25" t="str">
-        <f>_xlfn.CONCAT(D25," (",G25, ")")</f>
+        <f t="shared" si="0"/>
         <v>BAQ (Jet Fuel Diff – Singapore Jet Kerosene Cargoes (Platts) vs Singapore Gasoil 10 ppm (Platts) Future)</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1552,14 +1553,14 @@
         <v>33</v>
       </c>
       <c r="C26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Middle] ICEGO</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'GAS',</v>
       </c>
       <c r="F26" s="2">
@@ -1569,11 +1570,11 @@
         <v>93</v>
       </c>
       <c r="H26" t="str">
-        <f>_xlfn.CONCAT(D26," (",G26, ")")</f>
+        <f t="shared" si="0"/>
         <v>GAS (Low Sulphur Gasoil Futures)</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1581,14 +1582,14 @@
         <v>33</v>
       </c>
       <c r="C27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Middle] ICEGO</v>
       </c>
       <c r="D27" t="s">
         <v>35</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'ULA',</v>
       </c>
       <c r="F27">
@@ -1598,11 +1599,11 @@
         <v>94</v>
       </c>
       <c r="H27" t="str">
-        <f>_xlfn.CONCAT(D27," (",G27, ")")</f>
+        <f t="shared" si="0"/>
         <v>ULA (Low Sulphur Gasoil 1st Line Future)</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1610,14 +1611,14 @@
         <v>33</v>
       </c>
       <c r="C28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Middle] ICEGO</v>
       </c>
       <c r="D28" t="s">
         <v>36</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'ULD',</v>
       </c>
       <c r="F28">
@@ -1627,11 +1628,11 @@
         <v>95</v>
       </c>
       <c r="H28" t="str">
-        <f>_xlfn.CONCAT(D28," (",G28, ")")</f>
+        <f t="shared" si="0"/>
         <v>ULD (Gasoil Crack - Low Sulphur Gasoil 1st Line vs Brent 1st Line Future (in Bbls))</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1639,14 +1640,14 @@
         <v>33</v>
       </c>
       <c r="C29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Middle] ICEGO</v>
       </c>
       <c r="D29" t="s">
         <v>37</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'ULJ',</v>
       </c>
       <c r="F29">
@@ -1656,11 +1657,11 @@
         <v>96</v>
       </c>
       <c r="H29" t="str">
-        <f>_xlfn.CONCAT(D29," (",G29, ")")</f>
+        <f t="shared" si="0"/>
         <v>ULJ (Jet Fuel Diff - Jet CIF NWE Cargoes vs Low Sulphur Gasoil 1st Line Future)</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -1668,14 +1669,14 @@
         <v>33</v>
       </c>
       <c r="C30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Middle] ICEGO</v>
       </c>
       <c r="D30" t="s">
         <v>31</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'BAP',</v>
       </c>
       <c r="F30">
@@ -1685,11 +1686,11 @@
         <v>91</v>
       </c>
       <c r="H30" t="str">
-        <f>_xlfn.CONCAT(D30," (",G30, ")")</f>
+        <f t="shared" si="0"/>
         <v>BAP (Gasoil Diff - Singapore Gasoil (Platts) vs Low Sulphur Gasoil 1st Line Future (in Bbls))</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -1697,14 +1698,14 @@
         <v>33</v>
       </c>
       <c r="C31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Middle] ICEGO</v>
       </c>
       <c r="D31" t="s">
         <v>38</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'ULM',</v>
       </c>
       <c r="F31">
@@ -1714,11 +1715,11 @@
         <v>97</v>
       </c>
       <c r="H31" t="str">
-        <f>_xlfn.CONCAT(D31," (",G31, ")")</f>
+        <f t="shared" si="0"/>
         <v>ULM (Heating Oil Arb - Heating Oil 1st Line vs Low Sulphur Gasoil 1st Line Future (in Bbls))</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -1726,14 +1727,14 @@
         <v>39</v>
       </c>
       <c r="C32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Middle] SKO</v>
       </c>
       <c r="D32" t="s">
         <v>40</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'SRS',</v>
       </c>
       <c r="F32">
@@ -1743,11 +1744,11 @@
         <v>98</v>
       </c>
       <c r="H32" t="str">
-        <f>_xlfn.CONCAT(D32," (",G32, ")")</f>
+        <f t="shared" si="0"/>
         <v>SRS (Singapore Jet Kerosene Swap)</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -1755,14 +1756,14 @@
         <v>39</v>
       </c>
       <c r="C33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Middle] SKO</v>
       </c>
       <c r="D33" t="s">
         <v>41</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'SFF',</v>
       </c>
       <c r="F33">
@@ -1772,11 +1773,11 @@
         <v>99</v>
       </c>
       <c r="H33" t="str">
-        <f>_xlfn.CONCAT(D33," (",G33, ")")</f>
+        <f t="shared" si="0"/>
         <v>SFF (Jet Fuel Crack - Singapore Jet Kerosene Cargoes (Platts) vs Dubai 1st Line (Platts) Future)</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -1784,14 +1785,14 @@
         <v>39</v>
       </c>
       <c r="C34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Middle] SKO</v>
       </c>
       <c r="D34" t="s">
         <v>32</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'BAQ',</v>
       </c>
       <c r="F34">
@@ -1801,11 +1802,11 @@
         <v>92</v>
       </c>
       <c r="H34" t="str">
-        <f>_xlfn.CONCAT(D34," (",G34, ")")</f>
+        <f t="shared" ref="H34:H63" si="3">_xlfn.CONCAT(D34," (",G34, ")")</f>
         <v>BAQ (Jet Fuel Diff – Singapore Jet Kerosene Cargoes (Platts) vs Singapore Gasoil 10 ppm (Platts) Future)</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -1813,14 +1814,14 @@
         <v>42</v>
       </c>
       <c r="C35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Middle] NWE Jet</v>
       </c>
       <c r="D35" t="s">
         <v>43</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'JCN',</v>
       </c>
       <c r="F35">
@@ -1830,11 +1831,11 @@
         <v>100</v>
       </c>
       <c r="H35" t="str">
-        <f>_xlfn.CONCAT(D35," (",G35, ")")</f>
+        <f t="shared" si="3"/>
         <v>JCN (Jet CIF NWE Cargoes Future)</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -1842,14 +1843,14 @@
         <v>42</v>
       </c>
       <c r="C36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Middle] NWE Jet</v>
       </c>
       <c r="D36" t="s">
         <v>44</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'JNB',</v>
       </c>
       <c r="F36">
@@ -1859,11 +1860,11 @@
         <v>101</v>
       </c>
       <c r="H36" t="str">
-        <f>_xlfn.CONCAT(D36," (",G36, ")")</f>
+        <f t="shared" si="3"/>
         <v>JNB (Jet Fuel Crack - Jet CIF NWE Cargoes vs Brent 1st Line Future)</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>26</v>
       </c>
@@ -1871,14 +1872,14 @@
         <v>42</v>
       </c>
       <c r="C37" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Middle] NWE Jet</v>
       </c>
       <c r="D37" t="s">
         <v>37</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'ULJ',</v>
       </c>
       <c r="F37">
@@ -1888,11 +1889,11 @@
         <v>96</v>
       </c>
       <c r="H37" t="str">
-        <f>_xlfn.CONCAT(D37," (",G37, ")")</f>
+        <f t="shared" si="3"/>
         <v>ULJ (Jet Fuel Diff - Jet CIF NWE Cargoes vs Low Sulphur Gasoil 1st Line Future)</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>26</v>
       </c>
@@ -1900,14 +1901,14 @@
         <v>42</v>
       </c>
       <c r="C38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Middle] NWE Jet</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'JRJ',</v>
       </c>
       <c r="F38">
@@ -1917,11 +1918,11 @@
         <v>46</v>
       </c>
       <c r="H38" t="str">
-        <f>_xlfn.CONCAT(D38," (",G38, ")")</f>
+        <f t="shared" si="3"/>
         <v>JRJ (Jet Fuel Diff - Jet FOB Rotterdam Barges vs Jet CIF NWE Cargoes Future)</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>26</v>
       </c>
@@ -1929,14 +1930,14 @@
         <v>47</v>
       </c>
       <c r="C39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Middle] HO</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'UHO',</v>
       </c>
       <c r="F39" s="2">
@@ -1946,11 +1947,11 @@
         <v>102</v>
       </c>
       <c r="H39" t="str">
-        <f>_xlfn.CONCAT(D39," (",G39, ")")</f>
+        <f t="shared" si="3"/>
         <v>UHO (Heating Oil Futures)</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -1958,14 +1959,14 @@
         <v>47</v>
       </c>
       <c r="C40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Middle] HO</v>
       </c>
       <c r="D40" t="s">
         <v>49</v>
       </c>
       <c r="E40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'HOF',</v>
       </c>
       <c r="F40">
@@ -1975,11 +1976,11 @@
         <v>103</v>
       </c>
       <c r="H40" t="str">
-        <f>_xlfn.CONCAT(D40," (",G40, ")")</f>
+        <f t="shared" si="3"/>
         <v>HOF (Heating Oil 1st Line Future)</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>26</v>
       </c>
@@ -1987,14 +1988,14 @@
         <v>47</v>
       </c>
       <c r="C41" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Middle] HO</v>
       </c>
       <c r="D41" t="s">
         <v>50</v>
       </c>
       <c r="E41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'HBT',</v>
       </c>
       <c r="F41">
@@ -2004,11 +2005,11 @@
         <v>104</v>
       </c>
       <c r="H41" t="str">
-        <f>_xlfn.CONCAT(D41," (",G41, ")")</f>
+        <f t="shared" si="3"/>
         <v>HBT (Heating Oil Crack - Heating Oil 1st Line vs Brent 1st Line Future (in bbls))</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -2016,14 +2017,14 @@
         <v>47</v>
       </c>
       <c r="C42" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Middle] HO</v>
       </c>
       <c r="D42" t="s">
         <v>38</v>
       </c>
       <c r="E42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'ULM',</v>
       </c>
       <c r="F42">
@@ -2033,11 +2034,11 @@
         <v>97</v>
       </c>
       <c r="H42" t="str">
-        <f>_xlfn.CONCAT(D42," (",G42, ")")</f>
+        <f t="shared" si="3"/>
         <v>ULM (Heating Oil Arb - Heating Oil 1st Line vs Low Sulphur Gasoil 1st Line Future (in Bbls))</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -2045,14 +2046,14 @@
         <v>52</v>
       </c>
       <c r="C43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Heavy] S0.5</v>
       </c>
       <c r="D43" t="s">
         <v>53</v>
       </c>
       <c r="E43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'MF4',</v>
       </c>
       <c r="F43">
@@ -2062,11 +2063,11 @@
         <v>105</v>
       </c>
       <c r="H43" t="str">
-        <f>_xlfn.CONCAT(D43," (",G43, ")")</f>
+        <f t="shared" si="3"/>
         <v>MF4 (Marine Fuel 0.5% FOB Singapore Swap)</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -2074,14 +2075,14 @@
         <v>52</v>
       </c>
       <c r="C44" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Heavy] S0.5</v>
       </c>
       <c r="D44" t="s">
         <v>54</v>
       </c>
       <c r="E44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'MFT',</v>
       </c>
       <c r="F44">
@@ -2091,11 +2092,11 @@
         <v>106</v>
       </c>
       <c r="H44" t="str">
-        <f>_xlfn.CONCAT(D44," (",G44, ")")</f>
+        <f t="shared" si="3"/>
         <v>MFT (Fuel Oil Crack - Marine Fuel 0.5% FOB Singapore (Platts) vs Brent 1st Line Future (in Bbls))</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -2103,14 +2104,14 @@
         <v>52</v>
       </c>
       <c r="C45" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Heavy] S0.5</v>
       </c>
       <c r="D45" t="s">
         <v>55</v>
       </c>
       <c r="E45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'TEN',</v>
       </c>
       <c r="F45">
@@ -2120,11 +2121,11 @@
         <v>107</v>
       </c>
       <c r="H45" t="str">
-        <f>_xlfn.CONCAT(D45," (",G45, ")")</f>
+        <f t="shared" si="3"/>
         <v>TEN (Fuel Oil Crack - Marine Fuel 0.5% FOB Singapore (Platts) vs Brent 1st Line Future (in MTs))</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>51</v>
       </c>
@@ -2132,14 +2133,14 @@
         <v>52</v>
       </c>
       <c r="C46" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Heavy] S0.5</v>
       </c>
       <c r="D46" t="s">
         <v>56</v>
       </c>
       <c r="E46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'MF6',</v>
       </c>
       <c r="F46">
@@ -2149,11 +2150,11 @@
         <v>108</v>
       </c>
       <c r="H46" t="str">
-        <f>_xlfn.CONCAT(D46," (",G46, ")")</f>
+        <f t="shared" si="3"/>
         <v>MF6 (Fuel Oil Diff - Marine Fuel 0.5% FOB Singapore (Platts) vs 380 CST Singapore (Platts) Future)</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -2161,14 +2162,14 @@
         <v>52</v>
       </c>
       <c r="C47" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Heavy] S0.5</v>
       </c>
       <c r="D47" t="s">
         <v>57</v>
       </c>
       <c r="E47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'MF7',</v>
       </c>
       <c r="F47">
@@ -2178,11 +2179,11 @@
         <v>109</v>
       </c>
       <c r="H47" t="str">
-        <f>_xlfn.CONCAT(D47," (",G47, ")")</f>
+        <f t="shared" si="3"/>
         <v>MF7 (Fuel Oil Diff - Marine Fuel 0.5% FOB Singapore (Platts) vs Marine Fuel 0.5% FOB Rotterdam Barges (Platts) Futures)</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -2190,14 +2191,14 @@
         <v>52</v>
       </c>
       <c r="C48" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Heavy] S0.5</v>
       </c>
       <c r="D48" t="s">
         <v>58</v>
       </c>
       <c r="E48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'FDF',</v>
       </c>
       <c r="F48">
@@ -2207,11 +2208,11 @@
         <v>110</v>
       </c>
       <c r="H48" t="str">
-        <f>_xlfn.CONCAT(D48," (",G48, ")")</f>
+        <f t="shared" si="3"/>
         <v>FDF (Fuel Oil Diff - Marine Fuel 0.5% FOB Singapore (Platts) vs Singapore Gasoil (Platts) Future (in MTs))</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>51</v>
       </c>
@@ -2219,14 +2220,14 @@
         <v>59</v>
       </c>
       <c r="C49" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Heavy] Rdm0.5</v>
       </c>
       <c r="D49" t="s">
         <v>60</v>
       </c>
       <c r="E49" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'MF3',</v>
       </c>
       <c r="F49">
@@ -2236,11 +2237,11 @@
         <v>111</v>
       </c>
       <c r="H49" t="str">
-        <f>_xlfn.CONCAT(D49," (",G49, ")")</f>
+        <f t="shared" si="3"/>
         <v>MF3 (Marine Fuel 0.5% FOB Rotterdam Barge Swap)</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>51</v>
       </c>
@@ -2248,14 +2249,14 @@
         <v>59</v>
       </c>
       <c r="C50" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Heavy] Rdm0.5</v>
       </c>
       <c r="D50" t="s">
         <v>61</v>
       </c>
       <c r="E50" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'MF5',</v>
       </c>
       <c r="F50">
@@ -2265,11 +2266,11 @@
         <v>112</v>
       </c>
       <c r="H50" t="str">
-        <f>_xlfn.CONCAT(D50," (",G50, ")")</f>
+        <f t="shared" si="3"/>
         <v>MF5 (Marine Fuel 0.5% FOB Rotterdam Barges vs Fuel Oil 3.5% FOB Rotterdam Barges Swap)</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -2277,14 +2278,14 @@
         <v>59</v>
       </c>
       <c r="C51" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Heavy] Rdm0.5</v>
       </c>
       <c r="D51" t="s">
         <v>62</v>
       </c>
       <c r="E51" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'MFR',</v>
       </c>
       <c r="F51">
@@ -2294,11 +2295,11 @@
         <v>113</v>
       </c>
       <c r="H51" t="str">
-        <f>_xlfn.CONCAT(D51," (",G51, ")")</f>
+        <f t="shared" si="3"/>
         <v>MFR (Fuel Oil Crack - Marine Fuel 0.5% FOB Rotterdam Barges (Platts) vs Brent 1st Line Future (in Bbls))</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2306,14 +2307,14 @@
         <v>59</v>
       </c>
       <c r="C52" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Heavy] Rdm0.5</v>
       </c>
       <c r="D52" t="s">
         <v>63</v>
       </c>
       <c r="E52" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'TEO',</v>
       </c>
       <c r="F52">
@@ -2323,11 +2324,11 @@
         <v>114</v>
       </c>
       <c r="H52" t="str">
-        <f>_xlfn.CONCAT(D52," (",G52, ")")</f>
+        <f t="shared" si="3"/>
         <v>TEO (Fuel Oil Crack - Marine Fuel 0.5% FOB Rotterdam Barges (Platts) vs Brent 1st Line Future (in MTs))</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -2335,14 +2336,14 @@
         <v>59</v>
       </c>
       <c r="C53" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Heavy] Rdm0.5</v>
       </c>
       <c r="D53" t="s">
         <v>57</v>
       </c>
       <c r="E53" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'MF7',</v>
       </c>
       <c r="F53">
@@ -2352,11 +2353,11 @@
         <v>109</v>
       </c>
       <c r="H53" t="str">
-        <f>_xlfn.CONCAT(D53," (",G53, ")")</f>
+        <f t="shared" si="3"/>
         <v>MF7 (Fuel Oil Diff - Marine Fuel 0.5% FOB Singapore (Platts) vs Marine Fuel 0.5% FOB Rotterdam Barges (Platts) Futures)</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -2364,14 +2365,14 @@
         <v>64</v>
       </c>
       <c r="C54" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Heavy] S380</v>
       </c>
       <c r="D54" t="s">
         <v>65</v>
       </c>
       <c r="E54" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'SYS',</v>
       </c>
       <c r="F54">
@@ -2381,11 +2382,11 @@
         <v>115</v>
       </c>
       <c r="H54" t="str">
-        <f>_xlfn.CONCAT(D54," (",G54, ")")</f>
+        <f t="shared" si="3"/>
         <v>SYS (Fuel Oil 380 CST Singapore Swap)</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>51</v>
       </c>
@@ -2393,14 +2394,14 @@
         <v>64</v>
       </c>
       <c r="C55" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Heavy] S380</v>
       </c>
       <c r="D55" t="s">
         <v>66</v>
       </c>
       <c r="E55" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'SPS',</v>
       </c>
       <c r="F55">
@@ -2410,11 +2411,11 @@
         <v>116</v>
       </c>
       <c r="H55" t="str">
-        <f>_xlfn.CONCAT(D55," (",G55, ")")</f>
+        <f t="shared" si="3"/>
         <v>SPS (Fuel Oil Crack - Fuel Oil 380 CST Singapore vs Brent 1st Line Future)</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>51</v>
       </c>
@@ -2422,14 +2423,14 @@
         <v>64</v>
       </c>
       <c r="C56" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Heavy] S380</v>
       </c>
       <c r="D56" t="s">
         <v>67</v>
       </c>
       <c r="E56" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'SLS',</v>
       </c>
       <c r="F56">
@@ -2439,11 +2440,11 @@
         <v>117</v>
       </c>
       <c r="H56" t="str">
-        <f>_xlfn.CONCAT(D56," (",G56, ")")</f>
+        <f t="shared" si="3"/>
         <v>SLS (Fuel Oil Crack - Fuel Oil 380 CST Singapore vs Dubai 1st Line Future)</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>51</v>
       </c>
@@ -2451,14 +2452,14 @@
         <v>64</v>
       </c>
       <c r="C57" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Heavy] S380</v>
       </c>
       <c r="D57" t="s">
         <v>68</v>
       </c>
       <c r="E57" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'SJS',</v>
       </c>
       <c r="F57">
@@ -2468,11 +2469,11 @@
         <v>118</v>
       </c>
       <c r="H57" t="str">
-        <f>_xlfn.CONCAT(D57," (",G57, ")")</f>
+        <f t="shared" si="3"/>
         <v>SJS (Fuel Oil Diff - Fuel Oil 380 CST Singapore vs. 3.5% FOB Rotterdam Barges Swap)</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>51</v>
       </c>
@@ -2480,14 +2481,14 @@
         <v>64</v>
       </c>
       <c r="C58" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Heavy] S380</v>
       </c>
       <c r="D58" t="s">
         <v>56</v>
       </c>
       <c r="E58" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'MF6',</v>
       </c>
       <c r="F58">
@@ -2497,11 +2498,11 @@
         <v>108</v>
       </c>
       <c r="H58" t="str">
-        <f>_xlfn.CONCAT(D58," (",G58, ")")</f>
+        <f t="shared" si="3"/>
         <v>MF6 (Fuel Oil Diff - Marine Fuel 0.5% FOB Singapore (Platts) vs 380 CST Singapore (Platts) Future)</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>51</v>
       </c>
@@ -2509,14 +2510,14 @@
         <v>69</v>
       </c>
       <c r="C59" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Heavy] Rdm3.5</v>
       </c>
       <c r="D59" t="s">
         <v>70</v>
       </c>
       <c r="E59" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'BAR',</v>
       </c>
       <c r="F59">
@@ -2526,11 +2527,11 @@
         <v>119</v>
       </c>
       <c r="H59" t="str">
-        <f>_xlfn.CONCAT(D59," (",G59, ")")</f>
+        <f t="shared" si="3"/>
         <v>BAR (Fuel Oil 3.5% FOB Rotterdam Barges Balmo Swap)</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>51</v>
       </c>
@@ -2538,14 +2539,14 @@
         <v>69</v>
       </c>
       <c r="C60" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Heavy] Rdm3.5</v>
       </c>
       <c r="D60" t="s">
         <v>71</v>
       </c>
       <c r="E60" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'BOB',</v>
       </c>
       <c r="F60">
@@ -2555,11 +2556,11 @@
         <v>120</v>
       </c>
       <c r="H60" t="str">
-        <f>_xlfn.CONCAT(D60," (",G60, ")")</f>
+        <f t="shared" si="3"/>
         <v>BOB (Fuel Oil Crack - Fuel Oil 3.5% FOB Rotterdam Barges vs Brent 1st Line Future)</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>51</v>
       </c>
@@ -2567,14 +2568,14 @@
         <v>69</v>
       </c>
       <c r="C61" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Heavy] Rdm3.5</v>
       </c>
       <c r="D61" t="s">
         <v>72</v>
       </c>
       <c r="E61" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'BOA',</v>
       </c>
       <c r="F61">
@@ -2584,11 +2585,11 @@
         <v>121</v>
       </c>
       <c r="H61" t="str">
-        <f>_xlfn.CONCAT(D61," (",G61, ")")</f>
+        <f t="shared" si="3"/>
         <v>BOA (Fuel Oil Crack - Fuel Oil 3.5% FOB Rotterdam Barges vs Brent 1st Line Future (in Bbls))</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>51</v>
       </c>
@@ -2596,14 +2597,14 @@
         <v>69</v>
       </c>
       <c r="C62" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Heavy] Rdm3.5</v>
       </c>
       <c r="D62" t="s">
         <v>68</v>
       </c>
       <c r="E62" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'SJS',</v>
       </c>
       <c r="F62">
@@ -2613,11 +2614,11 @@
         <v>118</v>
       </c>
       <c r="H62" t="str">
-        <f>_xlfn.CONCAT(D62," (",G62, ")")</f>
+        <f t="shared" si="3"/>
         <v>SJS (Fuel Oil Diff - Fuel Oil 380 CST Singapore vs. 3.5% FOB Rotterdam Barges Swap)</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>51</v>
       </c>
@@ -2625,14 +2626,14 @@
         <v>69</v>
       </c>
       <c r="C63" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[Heavy] Rdm3.5</v>
       </c>
       <c r="D63" t="s">
         <v>61</v>
       </c>
       <c r="E63" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'MF5',</v>
       </c>
       <c r="F63">
@@ -2642,12 +2643,23 @@
         <v>112</v>
       </c>
       <c r="H63" t="str">
-        <f>_xlfn.CONCAT(D63," (",G63, ")")</f>
+        <f t="shared" si="3"/>
         <v>MF5 (Marine Fuel 0.5% FOB Rotterdam Barges vs Fuel Oil 3.5% FOB Rotterdam Barges Swap)</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H63" xr:uid="{54A59FE1-DE17-4881-8BC1-F91F83F8F9F7}"/>
+  <autoFilter ref="A1:H63" xr:uid="{54A59FE1-DE17-4881-8BC1-F91F83F8F9F7}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Light"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add summing OI conversions
</commit_message>
<xml_diff>
--- a/data/OI_product_map.xlsx
+++ b/data/OI_product_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hoteicapital-my.sharepoint.com/personal/jiashang_hoteicapital_com/Documents/Desktop/Notebooks/Streamlit_v1/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="257" documentId="8_{A4D98350-709A-462B-87D2-DA567DEA5457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1D36506-C0BA-402A-B611-B2FBE636F3E6}"/>
+  <xr:revisionPtr revIDLastSave="288" documentId="8_{A4D98350-709A-462B-87D2-DA567DEA5457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B77C7174-2A2C-46BE-8697-ECAA5D43490F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16080" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{542C41B4-5129-4961-BD89-52D58DBA0F0A}"/>
+    <workbookView xWindow="-120" yWindow="16080" windowWidth="38640" windowHeight="15840" xr2:uid="{542C41B4-5129-4961-BD89-52D58DBA0F0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$J$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$J$62</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet2!$A$1:$G$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="147">
   <si>
     <t>Product Family</t>
   </si>
@@ -185,9 +185,6 @@
     <t>JRJ</t>
   </si>
   <si>
-    <t>Jet Fuel Diff - Jet FOB Rotterdam Barges vs Jet CIF NWE Cargoes Future</t>
-  </si>
-  <si>
     <t>HO</t>
   </si>
   <si>
@@ -486,6 +483,9 @@
   </si>
   <si>
     <t>OI Unit</t>
+  </si>
+  <si>
+    <t>conversion_factor</t>
   </si>
 </sst>
 </file>
@@ -562,7 +562,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jia Shang" refreshedDate="45890.676370370369" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="62" xr:uid="{A8808549-A262-40B2-9E8C-C122B670117C}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:H63" sheet="Data"/>
+    <worksheetSource ref="A1:H62" sheet="Data"/>
   </cacheSource>
   <cacheFields count="8">
     <cacheField name="Product Family" numFmtId="0">
@@ -1831,10 +1831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A59FE1-DE17-4881-8BC1-F91F83F8F9F7}">
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6:J9"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1850,7 +1850,7 @@
     <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1858,31 +1858,34 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1904,7 +1907,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H2" t="str">
         <f t="shared" ref="H2:H33" si="0">_xlfn.CONCAT(D2," (",G2, ")")</f>
@@ -1918,8 +1921,11 @@
         <f>VLOOKUP(D2, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>BBL</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1927,21 +1933,21 @@
         <v>5</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C63" si="1">_xlfn.CONCAT("[",A3,"] ",B3)</f>
+        <f t="shared" ref="C3:C62" si="1">_xlfn.CONCAT("[",A3,"] ",B3)</f>
         <v>[Light] S92</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E63" si="2">_xlfn.CONCAT("'",D3,"',")</f>
+        <f t="shared" ref="E3:E62" si="2">_xlfn.CONCAT("'",D3,"',")</f>
         <v>'GDK',</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" si="0"/>
@@ -1955,8 +1961,11 @@
         <f>VLOOKUP(D3, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>BBL</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1978,7 +1987,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
@@ -1992,8 +2001,11 @@
         <f>VLOOKUP(D4, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>BBL</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2029,8 +2041,11 @@
         <f>VLOOKUP(D5, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2052,7 +2067,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
@@ -2066,8 +2081,11 @@
         <f>VLOOKUP(D6, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>BBL</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2089,7 +2107,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
@@ -2103,8 +2121,11 @@
         <f>VLOOKUP(D7, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -2126,7 +2147,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -2140,8 +2161,11 @@
         <f>VLOOKUP(D8, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2163,7 +2187,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -2177,8 +2201,11 @@
         <f>VLOOKUP(D9, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -2200,7 +2227,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
@@ -2214,8 +2241,11 @@
         <f>VLOOKUP(D10, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>BBL</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -2237,7 +2267,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
@@ -2251,8 +2281,11 @@
         <f>VLOOKUP(D11, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>BBL</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -2274,7 +2307,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
@@ -2288,8 +2321,11 @@
         <f>VLOOKUP(D12, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>BBL</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -2311,7 +2347,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
@@ -2325,8 +2361,11 @@
         <f>VLOOKUP(D13, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -2348,7 +2387,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -2362,8 +2401,11 @@
         <f>VLOOKUP(D14, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -2385,7 +2427,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -2399,8 +2441,11 @@
         <f>VLOOKUP(D15, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>BBL</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -2422,7 +2467,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
@@ -2436,8 +2481,11 @@
         <f>VLOOKUP(D16, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -2459,7 +2507,7 @@
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
@@ -2473,8 +2521,11 @@
         <f>VLOOKUP(D17, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -2496,7 +2547,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
@@ -2510,8 +2561,11 @@
         <f>VLOOKUP(D18, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -2533,7 +2587,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -2547,8 +2601,11 @@
         <f>VLOOKUP(D19, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -2570,7 +2627,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
@@ -2584,8 +2641,11 @@
         <f>VLOOKUP(D20, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -2607,7 +2667,7 @@
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
@@ -2621,8 +2681,11 @@
         <f>VLOOKUP(D21, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>BBL</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -2644,7 +2707,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
@@ -2658,8 +2721,11 @@
         <f>VLOOKUP(D22, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>BBL</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -2681,7 +2747,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
@@ -2695,8 +2761,11 @@
         <f>VLOOKUP(D23, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>BBL</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -2718,7 +2787,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
@@ -2732,8 +2801,11 @@
         <f>VLOOKUP(D24, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>BBL</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -2755,7 +2827,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
@@ -2769,8 +2841,11 @@
         <f>VLOOKUP(D25, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>BBL</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2792,7 +2867,7 @@
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
@@ -2806,8 +2881,11 @@
         <f>VLOOKUP(D26, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26">
+        <v>7.45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2829,7 +2907,7 @@
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
@@ -2843,8 +2921,11 @@
         <f>VLOOKUP(D27, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27">
+        <v>7.45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2866,7 +2947,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
@@ -2880,8 +2961,11 @@
         <f>VLOOKUP(D28, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>BBL</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -2903,7 +2987,7 @@
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
@@ -2917,8 +3001,11 @@
         <f>VLOOKUP(D29, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29">
+        <v>7.89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -2940,7 +3027,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
@@ -2954,8 +3041,11 @@
         <f>VLOOKUP(D30, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>BBL</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -2977,7 +3067,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
@@ -2991,8 +3081,11 @@
         <f>VLOOKUP(D31, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>BBL</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -3014,7 +3107,7 @@
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="0"/>
@@ -3028,8 +3121,11 @@
         <f>VLOOKUP(D32, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>BBL</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -3051,7 +3147,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="0"/>
@@ -3065,8 +3161,11 @@
         <f>VLOOKUP(D33, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>BBL</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -3088,10 +3187,10 @@
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" ref="H34:H63" si="3">_xlfn.CONCAT(D34," (",G34, ")")</f>
+        <f t="shared" ref="H34:H62" si="3">_xlfn.CONCAT(D34," (",G34, ")")</f>
         <v>BAQ (Jet Fuel Diff – Singapore Jet Kerosene Cargoes (Platts) vs Singapore Gasoil 10 ppm (Platts) Future)</v>
       </c>
       <c r="I34" t="str">
@@ -3102,8 +3201,11 @@
         <f>VLOOKUP(D34, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>BBL</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -3125,7 +3227,7 @@
         <v>1</v>
       </c>
       <c r="G35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="3"/>
@@ -3139,8 +3241,11 @@
         <f>VLOOKUP(D35, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K35">
+        <v>7.89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -3162,7 +3267,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="3"/>
@@ -3176,8 +3281,11 @@
         <f>VLOOKUP(D36, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>BBL</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>26</v>
       </c>
@@ -3199,7 +3307,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="3"/>
@@ -3213,50 +3321,56 @@
         <f>VLOOKUP(D37, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37">
+        <v>7.89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>26</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="1"/>
-        <v>[Middle] NWE Jet</v>
+        <v>[Middle] HO</v>
       </c>
       <c r="D38" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E38" t="str">
         <f t="shared" si="2"/>
-        <v>'JRJ',</v>
+        <v>'UHO',</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38" t="s">
-        <v>46</v>
+        <v>101</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="3"/>
-        <v>JRJ (Jet Fuel Diff - Jet FOB Rotterdam Barges vs Jet CIF NWE Cargoes Future)</v>
+        <v>UHO (Heating Oil Futures)</v>
       </c>
       <c r="I38" t="str">
         <f>VLOOKUP(D38, Sheet1!$A$4:$D$53, 4, FALSE)</f>
-        <v>$/MT</v>
+        <v>$/GAL</v>
       </c>
       <c r="J38" t="str">
         <f>VLOOKUP(D38, Sheet1!$A$4:$B$53, 2, FALSE)</f>
-        <v>MT</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <v>BBL</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="1"/>
@@ -3267,7 +3381,7 @@
       </c>
       <c r="E39" t="str">
         <f t="shared" si="2"/>
-        <v>'UHO',</v>
+        <v>'HOF',</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -3277,7 +3391,7 @@
       </c>
       <c r="H39" t="str">
         <f t="shared" si="3"/>
-        <v>UHO (Heating Oil Futures)</v>
+        <v>HOF (Heating Oil 1st Line Future)</v>
       </c>
       <c r="I39" t="str">
         <f>VLOOKUP(D39, Sheet1!$A$4:$D$53, 4, FALSE)</f>
@@ -3287,13 +3401,16 @@
         <f>VLOOKUP(D39, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>BBL</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="1"/>
@@ -3304,107 +3421,116 @@
       </c>
       <c r="E40" t="str">
         <f t="shared" si="2"/>
-        <v>'HOF',</v>
+        <v>'HBT',</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40" t="s">
         <v>103</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="3"/>
-        <v>HOF (Heating Oil 1st Line Future)</v>
+        <v>HBT (Heating Oil Crack - Heating Oil 1st Line vs Brent 1st Line Future (in bbls))</v>
       </c>
       <c r="I40" t="str">
         <f>VLOOKUP(D40, Sheet1!$A$4:$D$53, 4, FALSE)</f>
-        <v>$/GAL</v>
+        <v>$/BBL</v>
       </c>
       <c r="J40" t="str">
         <f>VLOOKUP(D40, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>BBL</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>26</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="1"/>
         <v>[Middle] HO</v>
       </c>
       <c r="D41" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" si="2"/>
-        <v>'HBT',</v>
+        <v>'ULM',</v>
       </c>
       <c r="F41">
         <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="3"/>
-        <v>HBT (Heating Oil Crack - Heating Oil 1st Line vs Brent 1st Line Future (in bbls))</v>
+        <v>ULM (Heating Oil Arb - Heating Oil 1st Line vs Low Sulphur Gasoil 1st Line Future (in Bbls))</v>
       </c>
       <c r="I41" t="str">
         <f>VLOOKUP(D41, Sheet1!$A$4:$D$53, 4, FALSE)</f>
-        <v>$/BBL</v>
+        <v>$/GAL</v>
       </c>
       <c r="J41" t="str">
         <f>VLOOKUP(D41, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>BBL</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B42" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="1"/>
-        <v>[Middle] HO</v>
+        <v>[Heavy] S0.5</v>
       </c>
       <c r="D42" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" si="2"/>
-        <v>'ULM',</v>
+        <v>'MF4',</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="3"/>
-        <v>ULM (Heating Oil Arb - Heating Oil 1st Line vs Low Sulphur Gasoil 1st Line Future (in Bbls))</v>
+        <v>MF4 (Marine Fuel 0.5% FOB Singapore Swap)</v>
       </c>
       <c r="I42" t="str">
         <f>VLOOKUP(D42, Sheet1!$A$4:$D$53, 4, FALSE)</f>
-        <v>$/GAL</v>
+        <v>$/MT</v>
       </c>
       <c r="J42" t="str">
         <f>VLOOKUP(D42, Sheet1!$A$4:$B$53, 2, FALSE)</f>
-        <v>BBL</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+        <v>MT</v>
+      </c>
+      <c r="K42">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" t="s">
         <v>51</v>
-      </c>
-      <c r="B43" t="s">
-        <v>52</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="1"/>
@@ -3415,33 +3541,36 @@
       </c>
       <c r="E43" t="str">
         <f t="shared" si="2"/>
-        <v>'MF4',</v>
+        <v>'MFT',</v>
       </c>
       <c r="F43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43" t="s">
         <v>105</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="3"/>
-        <v>MF4 (Marine Fuel 0.5% FOB Singapore Swap)</v>
+        <v>MFT (Fuel Oil Crack - Marine Fuel 0.5% FOB Singapore (Platts) vs Brent 1st Line Future (in Bbls))</v>
       </c>
       <c r="I43" t="str">
         <f>VLOOKUP(D43, Sheet1!$A$4:$D$53, 4, FALSE)</f>
-        <v>$/MT</v>
+        <v>$/BBL</v>
       </c>
       <c r="J43" t="str">
         <f>VLOOKUP(D43, Sheet1!$A$4:$B$53, 2, FALSE)</f>
-        <v>MT</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+        <v>BBL</v>
+      </c>
+      <c r="K43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" t="s">
         <v>51</v>
-      </c>
-      <c r="B44" t="s">
-        <v>52</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="1"/>
@@ -3452,7 +3581,7 @@
       </c>
       <c r="E44" t="str">
         <f t="shared" si="2"/>
-        <v>'MFT',</v>
+        <v>'TEN',</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -3462,7 +3591,7 @@
       </c>
       <c r="H44" t="str">
         <f t="shared" si="3"/>
-        <v>MFT (Fuel Oil Crack - Marine Fuel 0.5% FOB Singapore (Platts) vs Brent 1st Line Future (in Bbls))</v>
+        <v>TEN (Fuel Oil Crack - Marine Fuel 0.5% FOB Singapore (Platts) vs Brent 1st Line Future (in MTs))</v>
       </c>
       <c r="I44" t="str">
         <f>VLOOKUP(D44, Sheet1!$A$4:$D$53, 4, FALSE)</f>
@@ -3470,15 +3599,18 @@
       </c>
       <c r="J44" t="str">
         <f>VLOOKUP(D44, Sheet1!$A$4:$B$53, 2, FALSE)</f>
-        <v>BBL</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+        <v>MT</v>
+      </c>
+      <c r="K44">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" t="s">
         <v>51</v>
-      </c>
-      <c r="B45" t="s">
-        <v>52</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="1"/>
@@ -3489,7 +3621,7 @@
       </c>
       <c r="E45" t="str">
         <f t="shared" si="2"/>
-        <v>'TEN',</v>
+        <v>'MF6',</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -3499,23 +3631,26 @@
       </c>
       <c r="H45" t="str">
         <f t="shared" si="3"/>
-        <v>TEN (Fuel Oil Crack - Marine Fuel 0.5% FOB Singapore (Platts) vs Brent 1st Line Future (in MTs))</v>
+        <v>MF6 (Fuel Oil Diff - Marine Fuel 0.5% FOB Singapore (Platts) vs 380 CST Singapore (Platts) Future)</v>
       </c>
       <c r="I45" t="str">
         <f>VLOOKUP(D45, Sheet1!$A$4:$D$53, 4, FALSE)</f>
-        <v>$/BBL</v>
+        <v>$/MT</v>
       </c>
       <c r="J45" t="str">
         <f>VLOOKUP(D45, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K45">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46" t="s">
         <v>51</v>
-      </c>
-      <c r="B46" t="s">
-        <v>52</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="1"/>
@@ -3526,7 +3661,7 @@
       </c>
       <c r="E46" t="str">
         <f t="shared" si="2"/>
-        <v>'MF6',</v>
+        <v>'MF7',</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -3536,7 +3671,7 @@
       </c>
       <c r="H46" t="str">
         <f t="shared" si="3"/>
-        <v>MF6 (Fuel Oil Diff - Marine Fuel 0.5% FOB Singapore (Platts) vs 380 CST Singapore (Platts) Future)</v>
+        <v>MF7 (Fuel Oil Diff - Marine Fuel 0.5% FOB Singapore (Platts) vs Marine Fuel 0.5% FOB Rotterdam Barges (Platts) Futures)</v>
       </c>
       <c r="I46" t="str">
         <f>VLOOKUP(D46, Sheet1!$A$4:$D$53, 4, FALSE)</f>
@@ -3546,13 +3681,16 @@
         <f>VLOOKUP(D46, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K46">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" t="s">
         <v>51</v>
-      </c>
-      <c r="B47" t="s">
-        <v>52</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="1"/>
@@ -3563,7 +3701,7 @@
       </c>
       <c r="E47" t="str">
         <f t="shared" si="2"/>
-        <v>'MF7',</v>
+        <v>'FDF',</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -3573,7 +3711,7 @@
       </c>
       <c r="H47" t="str">
         <f t="shared" si="3"/>
-        <v>MF7 (Fuel Oil Diff - Marine Fuel 0.5% FOB Singapore (Platts) vs Marine Fuel 0.5% FOB Rotterdam Barges (Platts) Futures)</v>
+        <v>FDF (Fuel Oil Diff - Marine Fuel 0.5% FOB Singapore (Platts) vs Singapore Gasoil (Platts) Future (in MTs))</v>
       </c>
       <c r="I47" t="str">
         <f>VLOOKUP(D47, Sheet1!$A$4:$D$53, 4, FALSE)</f>
@@ -3583,34 +3721,37 @@
         <f>VLOOKUP(D47, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K47">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="1"/>
-        <v>[Heavy] S0.5</v>
+        <v>[Heavy] Rdm0.5</v>
       </c>
       <c r="D48" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" si="2"/>
-        <v>'FDF',</v>
+        <v>'MF3',</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48" t="s">
         <v>110</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" si="3"/>
-        <v>FDF (Fuel Oil Diff - Marine Fuel 0.5% FOB Singapore (Platts) vs Singapore Gasoil (Platts) Future (in MTs))</v>
+        <v>MF3 (Marine Fuel 0.5% FOB Rotterdam Barge Swap)</v>
       </c>
       <c r="I48" t="str">
         <f>VLOOKUP(D48, Sheet1!$A$4:$D$53, 4, FALSE)</f>
@@ -3620,13 +3761,16 @@
         <f>VLOOKUP(D48, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K48">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="1"/>
@@ -3637,17 +3781,17 @@
       </c>
       <c r="E49" t="str">
         <f t="shared" si="2"/>
-        <v>'MF3',</v>
+        <v>'MF5',</v>
       </c>
       <c r="F49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G49" t="s">
         <v>111</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="3"/>
-        <v>MF3 (Marine Fuel 0.5% FOB Rotterdam Barge Swap)</v>
+        <v>MF5 (Marine Fuel 0.5% FOB Rotterdam Barges vs Fuel Oil 3.5% FOB Rotterdam Barges Swap)</v>
       </c>
       <c r="I49" t="str">
         <f>VLOOKUP(D49, Sheet1!$A$4:$D$53, 4, FALSE)</f>
@@ -3657,13 +3801,16 @@
         <f>VLOOKUP(D49, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K49">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="1"/>
@@ -3674,7 +3821,7 @@
       </c>
       <c r="E50" t="str">
         <f t="shared" si="2"/>
-        <v>'MF5',</v>
+        <v>'MFR',</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -3684,23 +3831,26 @@
       </c>
       <c r="H50" t="str">
         <f t="shared" si="3"/>
-        <v>MF5 (Marine Fuel 0.5% FOB Rotterdam Barges vs Fuel Oil 3.5% FOB Rotterdam Barges Swap)</v>
+        <v>MFR (Fuel Oil Crack - Marine Fuel 0.5% FOB Rotterdam Barges (Platts) vs Brent 1st Line Future (in Bbls))</v>
       </c>
       <c r="I50" t="str">
         <f>VLOOKUP(D50, Sheet1!$A$4:$D$53, 4, FALSE)</f>
-        <v>$/MT</v>
+        <v>$/BBL</v>
       </c>
       <c r="J50" t="str">
         <f>VLOOKUP(D50, Sheet1!$A$4:$B$53, 2, FALSE)</f>
-        <v>MT</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+        <v>BBL</v>
+      </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="1"/>
@@ -3711,7 +3861,7 @@
       </c>
       <c r="E51" t="str">
         <f t="shared" si="2"/>
-        <v>'MFR',</v>
+        <v>'TEO',</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -3721,7 +3871,7 @@
       </c>
       <c r="H51" t="str">
         <f t="shared" si="3"/>
-        <v>MFR (Fuel Oil Crack - Marine Fuel 0.5% FOB Rotterdam Barges (Platts) vs Brent 1st Line Future (in Bbls))</v>
+        <v>TEO (Fuel Oil Crack - Marine Fuel 0.5% FOB Rotterdam Barges (Platts) vs Brent 1st Line Future (in MTs))</v>
       </c>
       <c r="I51" t="str">
         <f>VLOOKUP(D51, Sheet1!$A$4:$D$53, 4, FALSE)</f>
@@ -3729,73 +3879,79 @@
       </c>
       <c r="J51" t="str">
         <f>VLOOKUP(D51, Sheet1!$A$4:$B$53, 2, FALSE)</f>
-        <v>BBL</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+        <v>MT</v>
+      </c>
+      <c r="K51">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="1"/>
         <v>[Heavy] Rdm0.5</v>
       </c>
       <c r="D52" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E52" t="str">
         <f t="shared" si="2"/>
-        <v>'TEO',</v>
+        <v>'MF7',</v>
       </c>
       <c r="F52">
         <v>0</v>
       </c>
       <c r="G52" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="H52" t="str">
         <f t="shared" si="3"/>
-        <v>TEO (Fuel Oil Crack - Marine Fuel 0.5% FOB Rotterdam Barges (Platts) vs Brent 1st Line Future (in MTs))</v>
+        <v>MF7 (Fuel Oil Diff - Marine Fuel 0.5% FOB Singapore (Platts) vs Marine Fuel 0.5% FOB Rotterdam Barges (Platts) Futures)</v>
       </c>
       <c r="I52" t="str">
         <f>VLOOKUP(D52, Sheet1!$A$4:$D$53, 4, FALSE)</f>
-        <v>$/BBL</v>
+        <v>$/MT</v>
       </c>
       <c r="J52" t="str">
         <f>VLOOKUP(D52, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K52">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="1"/>
-        <v>[Heavy] Rdm0.5</v>
+        <v>[Heavy] S380</v>
       </c>
       <c r="D53" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E53" t="str">
         <f t="shared" si="2"/>
-        <v>'MF7',</v>
+        <v>'SYS',</v>
       </c>
       <c r="F53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="H53" t="str">
         <f t="shared" si="3"/>
-        <v>MF7 (Fuel Oil Diff - Marine Fuel 0.5% FOB Singapore (Platts) vs Marine Fuel 0.5% FOB Rotterdam Barges (Platts) Futures)</v>
+        <v>SYS (Fuel Oil 380 CST Singapore Swap)</v>
       </c>
       <c r="I53" t="str">
         <f>VLOOKUP(D53, Sheet1!$A$4:$D$53, 4, FALSE)</f>
@@ -3805,13 +3961,16 @@
         <f>VLOOKUP(D53, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K53">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="1"/>
@@ -3822,33 +3981,36 @@
       </c>
       <c r="E54" t="str">
         <f t="shared" si="2"/>
-        <v>'SYS',</v>
+        <v>'SPS',</v>
       </c>
       <c r="F54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G54" t="s">
         <v>115</v>
       </c>
       <c r="H54" t="str">
         <f t="shared" si="3"/>
-        <v>SYS (Fuel Oil 380 CST Singapore Swap)</v>
+        <v>SPS (Fuel Oil Crack - Fuel Oil 380 CST Singapore vs Brent 1st Line Future)</v>
       </c>
       <c r="I54" t="str">
         <f>VLOOKUP(D54, Sheet1!$A$4:$D$53, 4, FALSE)</f>
-        <v>$/MT</v>
+        <v>$/BBL</v>
       </c>
       <c r="J54" t="str">
         <f>VLOOKUP(D54, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K54">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="1"/>
@@ -3859,7 +4021,7 @@
       </c>
       <c r="E55" t="str">
         <f t="shared" si="2"/>
-        <v>'SPS',</v>
+        <v>'SLS',</v>
       </c>
       <c r="F55">
         <v>0</v>
@@ -3869,7 +4031,7 @@
       </c>
       <c r="H55" t="str">
         <f t="shared" si="3"/>
-        <v>SPS (Fuel Oil Crack - Fuel Oil 380 CST Singapore vs Brent 1st Line Future)</v>
+        <v>SLS (Fuel Oil Crack - Fuel Oil 380 CST Singapore vs Dubai 1st Line Future)</v>
       </c>
       <c r="I55" t="str">
         <f>VLOOKUP(D55, Sheet1!$A$4:$D$53, 4, FALSE)</f>
@@ -3879,13 +4041,16 @@
         <f>VLOOKUP(D55, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K55">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="1"/>
@@ -3896,7 +4061,7 @@
       </c>
       <c r="E56" t="str">
         <f t="shared" si="2"/>
-        <v>'SLS',</v>
+        <v>'SJS',</v>
       </c>
       <c r="F56">
         <v>0</v>
@@ -3906,44 +4071,47 @@
       </c>
       <c r="H56" t="str">
         <f t="shared" si="3"/>
-        <v>SLS (Fuel Oil Crack - Fuel Oil 380 CST Singapore vs Dubai 1st Line Future)</v>
+        <v>SJS (Fuel Oil Diff - Fuel Oil 380 CST Singapore vs. 3.5% FOB Rotterdam Barges Swap)</v>
       </c>
       <c r="I56" t="str">
         <f>VLOOKUP(D56, Sheet1!$A$4:$D$53, 4, FALSE)</f>
-        <v>$/BBL</v>
+        <v>$/MT</v>
       </c>
       <c r="J56" t="str">
         <f>VLOOKUP(D56, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K56">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B57" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="1"/>
         <v>[Heavy] S380</v>
       </c>
       <c r="D57" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="E57" t="str">
         <f t="shared" si="2"/>
-        <v>'SJS',</v>
+        <v>'MF6',</v>
       </c>
       <c r="F57">
         <v>0</v>
       </c>
       <c r="G57" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="H57" t="str">
         <f t="shared" si="3"/>
-        <v>SJS (Fuel Oil Diff - Fuel Oil 380 CST Singapore vs. 3.5% FOB Rotterdam Barges Swap)</v>
+        <v>MF6 (Fuel Oil Diff - Marine Fuel 0.5% FOB Singapore (Platts) vs 380 CST Singapore (Platts) Future)</v>
       </c>
       <c r="I57" t="str">
         <f>VLOOKUP(D57, Sheet1!$A$4:$D$53, 4, FALSE)</f>
@@ -3953,34 +4121,37 @@
         <f>VLOOKUP(D57, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K57">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B58" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="1"/>
-        <v>[Heavy] S380</v>
+        <v>[Heavy] Rdm3.5</v>
       </c>
       <c r="D58" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="E58" t="str">
         <f t="shared" si="2"/>
-        <v>'MF6',</v>
+        <v>'BAR',</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G58" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="H58" t="str">
         <f t="shared" si="3"/>
-        <v>MF6 (Fuel Oil Diff - Marine Fuel 0.5% FOB Singapore (Platts) vs 380 CST Singapore (Platts) Future)</v>
+        <v>BAR (Fuel Oil 3.5% FOB Rotterdam Barges Balmo Swap)</v>
       </c>
       <c r="I58" t="str">
         <f>VLOOKUP(D58, Sheet1!$A$4:$D$53, 4, FALSE)</f>
@@ -3990,13 +4161,16 @@
         <f>VLOOKUP(D58, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K58">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B59" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="1"/>
@@ -4007,33 +4181,36 @@
       </c>
       <c r="E59" t="str">
         <f t="shared" si="2"/>
-        <v>'BAR',</v>
+        <v>'BOB',</v>
       </c>
       <c r="F59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G59" t="s">
         <v>119</v>
       </c>
       <c r="H59" t="str">
         <f t="shared" si="3"/>
-        <v>BAR (Fuel Oil 3.5% FOB Rotterdam Barges Balmo Swap)</v>
+        <v>BOB (Fuel Oil Crack - Fuel Oil 3.5% FOB Rotterdam Barges vs Brent 1st Line Future)</v>
       </c>
       <c r="I59" t="str">
         <f>VLOOKUP(D59, Sheet1!$A$4:$D$53, 4, FALSE)</f>
-        <v>$/MT</v>
+        <v>$/BBL</v>
       </c>
       <c r="J59" t="str">
         <f>VLOOKUP(D59, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K59">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="1"/>
@@ -4044,7 +4221,7 @@
       </c>
       <c r="E60" t="str">
         <f t="shared" si="2"/>
-        <v>'BOB',</v>
+        <v>'BOA',</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -4054,7 +4231,7 @@
       </c>
       <c r="H60" t="str">
         <f t="shared" si="3"/>
-        <v>BOB (Fuel Oil Crack - Fuel Oil 3.5% FOB Rotterdam Barges vs Brent 1st Line Future)</v>
+        <v>BOA (Fuel Oil Crack - Fuel Oil 3.5% FOB Rotterdam Barges vs Brent 1st Line Future (in Bbls))</v>
       </c>
       <c r="I60" t="str">
         <f>VLOOKUP(D60, Sheet1!$A$4:$D$53, 4, FALSE)</f>
@@ -4062,73 +4239,79 @@
       </c>
       <c r="J60" t="str">
         <f>VLOOKUP(D60, Sheet1!$A$4:$B$53, 2, FALSE)</f>
-        <v>MT</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+        <v>BBL</v>
+      </c>
+      <c r="K60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B61" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="1"/>
         <v>[Heavy] Rdm3.5</v>
       </c>
       <c r="D61" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E61" t="str">
         <f t="shared" si="2"/>
-        <v>'BOA',</v>
+        <v>'SJS',</v>
       </c>
       <c r="F61">
         <v>0</v>
       </c>
       <c r="G61" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H61" t="str">
         <f t="shared" si="3"/>
-        <v>BOA (Fuel Oil Crack - Fuel Oil 3.5% FOB Rotterdam Barges vs Brent 1st Line Future (in Bbls))</v>
+        <v>SJS (Fuel Oil Diff - Fuel Oil 380 CST Singapore vs. 3.5% FOB Rotterdam Barges Swap)</v>
       </c>
       <c r="I61" t="str">
         <f>VLOOKUP(D61, Sheet1!$A$4:$D$53, 4, FALSE)</f>
-        <v>$/BBL</v>
+        <v>$/MT</v>
       </c>
       <c r="J61" t="str">
         <f>VLOOKUP(D61, Sheet1!$A$4:$B$53, 2, FALSE)</f>
-        <v>BBL</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+        <v>MT</v>
+      </c>
+      <c r="K61">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B62" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="1"/>
         <v>[Heavy] Rdm3.5</v>
       </c>
       <c r="D62" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E62" t="str">
         <f t="shared" si="2"/>
-        <v>'SJS',</v>
+        <v>'MF5',</v>
       </c>
       <c r="F62">
         <v>0</v>
       </c>
       <c r="G62" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="H62" t="str">
         <f t="shared" si="3"/>
-        <v>SJS (Fuel Oil Diff - Fuel Oil 380 CST Singapore vs. 3.5% FOB Rotterdam Barges Swap)</v>
+        <v>MF5 (Marine Fuel 0.5% FOB Rotterdam Barges vs Fuel Oil 3.5% FOB Rotterdam Barges Swap)</v>
       </c>
       <c r="I62" t="str">
         <f>VLOOKUP(D62, Sheet1!$A$4:$D$53, 4, FALSE)</f>
@@ -4138,46 +4321,12 @@
         <f>VLOOKUP(D62, Sheet1!$A$4:$B$53, 2, FALSE)</f>
         <v>MT</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>51</v>
-      </c>
-      <c r="B63" t="s">
-        <v>69</v>
-      </c>
-      <c r="C63" t="str">
-        <f t="shared" si="1"/>
-        <v>[Heavy] Rdm3.5</v>
-      </c>
-      <c r="D63" t="s">
-        <v>61</v>
-      </c>
-      <c r="E63" t="str">
-        <f t="shared" si="2"/>
-        <v>'MF5',</v>
-      </c>
-      <c r="F63">
-        <v>0</v>
-      </c>
-      <c r="G63" t="s">
-        <v>112</v>
-      </c>
-      <c r="H63" t="str">
-        <f t="shared" si="3"/>
-        <v>MF5 (Marine Fuel 0.5% FOB Rotterdam Barges vs Fuel Oil 3.5% FOB Rotterdam Barges Swap)</v>
-      </c>
-      <c r="I63" t="str">
-        <f>VLOOKUP(D63, Sheet1!$A$4:$D$53, 4, FALSE)</f>
-        <v>$/MT</v>
-      </c>
-      <c r="J63" t="str">
-        <f>VLOOKUP(D63, Sheet1!$A$4:$B$53, 2, FALSE)</f>
-        <v>MT</v>
+      <c r="K62">
+        <v>6.35</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J63" xr:uid="{54A59FE1-DE17-4881-8BC1-F91F83F8F9F7}"/>
+  <autoFilter ref="A1:J62" xr:uid="{54A59FE1-DE17-4881-8BC1-F91F83F8F9F7}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4200,23 +4349,23 @@
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G3" t="s">
         <v>126</v>
-      </c>
-      <c r="G3" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -4224,13 +4373,13 @@
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E4" s="2" t="b">
         <f t="shared" ref="E4:E35" si="0">B4=C4</f>
@@ -4242,13 +4391,13 @@
         <v>30</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E5" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4260,20 +4409,20 @@
         <v>31</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E6" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E6" s="2" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -4281,13 +4430,13 @@
         <v>32</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E7" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4296,16 +4445,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E8" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4314,16 +4463,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E9" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4332,23 +4481,23 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E10" s="2" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -4356,20 +4505,20 @@
         <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E11" s="2" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -4377,13 +4526,13 @@
         <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E12" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4392,16 +4541,16 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E13" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4416,13 +4565,13 @@
         <v>34</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E14" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4434,13 +4583,13 @@
         <v>7</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E15" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4452,20 +4601,20 @@
         <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E16" s="2" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4473,13 +4622,13 @@
         <v>28</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E17" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4488,16 +4637,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E18" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4506,23 +4655,23 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E19" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E19" s="2" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -4530,13 +4679,13 @@
         <v>43</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E20" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4548,13 +4697,13 @@
         <v>44</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E21" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4566,13 +4715,13 @@
         <v>22</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E22" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4584,13 +4733,13 @@
         <v>45</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E23" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4599,16 +4748,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E24" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4617,16 +4766,16 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E25" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4635,16 +4784,16 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E26" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4653,16 +4802,16 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E27" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4671,16 +4820,16 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E28" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4689,16 +4838,16 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E29" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4707,16 +4856,16 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E30" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4728,13 +4877,13 @@
         <v>21</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E31" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4746,13 +4895,13 @@
         <v>24</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E32" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4764,13 +4913,13 @@
         <v>20</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E33" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4782,20 +4931,20 @@
         <v>25</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E34" s="2" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -4803,13 +4952,13 @@
         <v>18</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E35" s="2" t="b">
         <f t="shared" si="0"/>
@@ -4821,20 +4970,20 @@
         <v>17</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E36" s="2" t="b">
         <f t="shared" ref="E36:E53" si="1">B36=C36</f>
         <v>0</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -4842,13 +4991,13 @@
         <v>41</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E37" s="2" t="b">
         <f t="shared" si="1"/>
@@ -4860,13 +5009,13 @@
         <v>29</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E38" s="2" t="b">
         <f t="shared" si="1"/>
@@ -4875,16 +5024,16 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E39" s="2" t="b">
         <f t="shared" si="1"/>
@@ -4893,23 +5042,23 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E40" s="2" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -4917,13 +5066,13 @@
         <v>6</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E41" s="2" t="b">
         <f t="shared" si="1"/>
@@ -4932,23 +5081,23 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E42" s="2" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -4956,13 +5105,13 @@
         <v>40</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E43" s="2" t="b">
         <f t="shared" si="1"/>
@@ -4974,13 +5123,13 @@
         <v>8</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E44" s="2" t="b">
         <f t="shared" si="1"/>
@@ -4989,16 +5138,16 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E45" s="2" t="b">
         <f t="shared" si="1"/>
@@ -5007,65 +5156,65 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E46" s="2" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E47" s="2" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C48" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E48" s="2" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E48" s="2" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -5073,20 +5222,20 @@
         <v>16</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C49" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E49" s="2" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F49" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E49" s="2" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -5094,13 +5243,13 @@
         <v>35</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E50" s="2" t="b">
         <f t="shared" si="1"/>
@@ -5112,13 +5261,13 @@
         <v>36</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E51" s="2" t="b">
         <f t="shared" si="1"/>
@@ -5130,13 +5279,13 @@
         <v>37</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E52" s="2" t="b">
         <f t="shared" si="1"/>
@@ -5148,25 +5297,25 @@
         <v>38</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C53" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E53" s="2" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E53" s="2" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -5183,8 +5332,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5200,22 +5349,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" t="s">
         <v>128</v>
       </c>
-      <c r="C1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D1" t="s">
-        <v>129</v>
-      </c>
       <c r="F1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" t="s">
         <v>126</v>
-      </c>
-      <c r="G1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -5223,13 +5372,13 @@
         <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E2" s="2" t="b">
         <f t="shared" ref="E2:E51" si="0">B2=C2</f>
@@ -5241,13 +5390,13 @@
         <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E3" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5259,20 +5408,20 @@
         <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E4" s="2" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -5280,13 +5429,13 @@
         <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E5" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5295,16 +5444,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E6" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5313,16 +5462,16 @@
     </row>
     <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E7" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5331,23 +5480,23 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E8" s="2" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -5355,20 +5504,20 @@
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E9" s="2" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -5376,13 +5525,13 @@
         <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E10" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5391,16 +5540,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E11" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5415,13 +5564,13 @@
         <v>34</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E12" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5433,13 +5582,13 @@
         <v>7</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E13" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5451,20 +5600,20 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E14" s="2" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -5472,13 +5621,13 @@
         <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E15" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5487,16 +5636,16 @@
     </row>
     <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E16" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5505,23 +5654,23 @@
     </row>
     <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E17" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E17" s="2" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -5529,13 +5678,13 @@
         <v>43</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E18" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5547,13 +5696,13 @@
         <v>44</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E19" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5565,13 +5714,13 @@
         <v>22</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E20" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5583,13 +5732,13 @@
         <v>45</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E21" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5598,16 +5747,16 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E22" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5616,16 +5765,16 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E23" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5634,16 +5783,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E24" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5652,16 +5801,16 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E25" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5670,16 +5819,16 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E26" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5688,16 +5837,16 @@
     </row>
     <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E27" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5706,16 +5855,16 @@
     </row>
     <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E28" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5727,13 +5876,13 @@
         <v>21</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E29" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5745,13 +5894,13 @@
         <v>24</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E30" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5763,13 +5912,13 @@
         <v>20</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E31" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5781,20 +5930,20 @@
         <v>25</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E32" s="2" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5802,13 +5951,13 @@
         <v>18</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E33" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5820,20 +5969,20 @@
         <v>17</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E34" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E34" s="2" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5841,13 +5990,13 @@
         <v>41</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E35" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5859,13 +6008,13 @@
         <v>29</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E36" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5874,16 +6023,16 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E37" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5892,23 +6041,23 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E38" s="2" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5916,13 +6065,13 @@
         <v>6</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E39" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5931,23 +6080,23 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E40" s="2" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5955,13 +6104,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E41" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5973,13 +6122,13 @@
         <v>8</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E42" s="2" t="b">
         <f t="shared" si="0"/>
@@ -5988,16 +6137,16 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E43" s="2" t="b">
         <f t="shared" si="0"/>
@@ -6006,65 +6155,65 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E44" s="2" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E45" s="2" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C46" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E46" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F46" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E46" s="2" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -6072,20 +6221,20 @@
         <v>16</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C47" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E47" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E47" s="2" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -6093,13 +6242,13 @@
         <v>35</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E48" s="2" t="b">
         <f t="shared" si="0"/>
@@ -6111,13 +6260,13 @@
         <v>36</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E49" s="2" t="b">
         <f t="shared" si="0"/>
@@ -6129,13 +6278,13 @@
         <v>37</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E50" s="2" t="b">
         <f t="shared" si="0"/>
@@ -6147,20 +6296,20 @@
         <v>38</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C51" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E51" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E51" s="2" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>